<commit_message>
Add necessary files and documentation for Python automation examples
- Created relatorio_2.xlsx and relatorio_3.xlsx in relatorios_diarios directory.
- Added arquivos_necessarios.md to document required files for executing examples.
- Introduced cronograma.md to outline study schedule for Python automation projects.
</commit_message>
<xml_diff>
--- a/codes/relatorio_vendas.xlsx
+++ b/codes/relatorio_vendas.xlsx
@@ -1,92 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian Mulato\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64130597-C4F4-403C-9D77-0612F903D441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Vendas" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>produto</t>
-  </si>
-  <si>
-    <t>quantidade</t>
-  </si>
-  <si>
-    <t>preco_unitario</t>
-  </si>
-  <si>
-    <t>total_venda</t>
-  </si>
-  <si>
-    <t>2025-06-01</t>
-  </si>
-  <si>
-    <t>2025-06-02</t>
-  </si>
-  <si>
-    <t>2025-06-03</t>
-  </si>
-  <si>
-    <t>2025-06-04</t>
-  </si>
-  <si>
-    <t>2025-06-05</t>
-  </si>
-  <si>
-    <t>Teclado</t>
-  </si>
-  <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>Monitor</t>
-  </si>
-  <si>
-    <t>Headset</t>
-  </si>
-  <si>
-    <t>Webcam</t>
-  </si>
-  <si>
-    <t>Impressora</t>
-  </si>
-  <si>
-    <t>Mousepad</t>
-  </si>
-  <si>
-    <t>Notebook</t>
-  </si>
-  <si>
-    <t>Fonte</t>
-  </si>
-  <si>
-    <t>Cabo HDMI</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>ID_Venda</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Valor_Unitario</t>
+  </si>
+  <si>
+    <t>2024-06-01</t>
+  </si>
+  <si>
+    <t>2024-06-02</t>
+  </si>
+  <si>
+    <t>2024-06-03</t>
+  </si>
+  <si>
+    <t>2024-06-04</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Caneta</t>
+  </si>
+  <si>
+    <t>Caderno</t>
+  </si>
+  <si>
+    <t>Mochila</t>
+  </si>
+  <si>
+    <t>Lápis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,21 +137,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +181,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -235,7 +215,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -270,10 +249,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,23 +424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,175 +447,88 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
+      <c r="F3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
         <v>150</v>
       </c>
-      <c r="E2">
-        <v>450</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>80</v>
-      </c>
-      <c r="E3">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>950</v>
-      </c>
-      <c r="E4">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>1004</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>200</v>
+      <c r="D5" t="s">
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="F5">
         <v>1</v>
-      </c>
-      <c r="D6">
-        <v>350</v>
-      </c>
-      <c r="E6">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>1200</v>
-      </c>
-      <c r="E7">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>4500</v>
-      </c>
-      <c r="E9">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>250</v>
-      </c>
-      <c r="E10">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>60</v>
-      </c>
-      <c r="E11">
-        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>